<commit_message>
Chapter 4 advanced. Finished the intermitent items
</commit_message>
<xml_diff>
--- a/bip8013_015_data.xlsx
+++ b/bip8013_015_data.xlsx
@@ -14,16 +14,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
   <si>
     <t>X</t>
   </si>
@@ -161,13 +157,43 @@
   </si>
   <si>
     <t>20-Nov</t>
+  </si>
+  <si>
+    <t>SES</t>
+  </si>
+  <si>
+    <t>Croston</t>
+  </si>
+  <si>
+    <t>SBA</t>
+  </si>
+  <si>
+    <t>SBJ</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>Error size</t>
+  </si>
+  <si>
+    <t>RMSE variation</t>
+  </si>
+  <si>
+    <t>MAE variation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +203,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -201,17 +234,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1975,820 +2019,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="0.1"/>
-      <sheetName val="0.15"/>
-      <sheetName val="0.5"/>
-      <sheetName val="optimal"/>
-      <sheetName val="interdemand inter."/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>BIP001271</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>Dec-17</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>Jan-18</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>Feb-18</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>Mar-18</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>Apr-18</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>May-18</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>Jun-18</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>Jul-18</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>Aug-18</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>Sep-18</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>Oct-18</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>Nov-18</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>Dec-18</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15" t="str">
-            <v>Jan-19</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16" t="str">
-            <v>Feb-19</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17" t="str">
-            <v>Mar-19</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18" t="str">
-            <v>Apr-19</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19" t="str">
-            <v>May-19</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20" t="str">
-            <v>Jun-19</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21" t="str">
-            <v>Jul-19</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22" t="str">
-            <v>Aug-19</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23" t="str">
-            <v>Sep-19</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24" t="str">
-            <v>Oct-19</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25" t="str">
-            <v>Nov-19</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26" t="str">
-            <v>Dec-19</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27" t="str">
-            <v>Jan-20</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28" t="str">
-            <v>Feb-20</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29" t="str">
-            <v>Mar-20</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30" t="str">
-            <v>Apr-20</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31" t="str">
-            <v>May-20</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32" t="str">
-            <v>Jun-20</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33" t="str">
-            <v>Jul-20</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34" t="str">
-            <v>Aug-20</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35" t="str">
-            <v>Sep-20</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36" t="str">
-            <v>Oct-20</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="A37" t="str">
-            <v>Nov-20</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>BIP008013</v>
-          </cell>
-          <cell r="C1" t="str">
-            <v>SES_bip8013</v>
-          </cell>
-          <cell r="D1" t="str">
-            <v>cros_smoothed</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>SBA_smoothed</v>
-          </cell>
-          <cell r="F1" t="str">
-            <v>SBJ_smoothed</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="B2">
-            <v>0</v>
-          </cell>
-          <cell r="C2">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3">
-            <v>0</v>
-          </cell>
-          <cell r="C3">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4">
-            <v>0</v>
-          </cell>
-          <cell r="C4">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5">
-            <v>0</v>
-          </cell>
-          <cell r="C5">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>0</v>
-          </cell>
-          <cell r="C6">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7">
-            <v>0</v>
-          </cell>
-          <cell r="C7">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8">
-            <v>0</v>
-          </cell>
-          <cell r="C8">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9">
-            <v>0</v>
-          </cell>
-          <cell r="C9">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10">
-            <v>0</v>
-          </cell>
-          <cell r="C10">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11">
-            <v>0</v>
-          </cell>
-          <cell r="C11">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12">
-            <v>0</v>
-          </cell>
-          <cell r="C12">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13">
-            <v>5</v>
-          </cell>
-          <cell r="C13">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14">
-            <v>5480</v>
-          </cell>
-          <cell r="C14">
-            <v>0.5</v>
-          </cell>
-          <cell r="D14">
-            <v>421.92195390909211</v>
-          </cell>
-          <cell r="E14">
-            <v>421.91850799434349</v>
-          </cell>
-          <cell r="F14">
-            <v>421.92280809939558</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15">
-            <v>0</v>
-          </cell>
-          <cell r="C15">
-            <v>548.45000000000005</v>
-          </cell>
-          <cell r="D15">
-            <v>557.14954360648824</v>
-          </cell>
-          <cell r="E15">
-            <v>562.16245604034521</v>
-          </cell>
-          <cell r="F15">
-            <v>562.45612196622142</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16">
-            <v>0</v>
-          </cell>
-          <cell r="C16">
-            <v>493.60500000000008</v>
-          </cell>
-          <cell r="D16">
-            <v>557.14954360648824</v>
-          </cell>
-          <cell r="E16">
-            <v>562.16245604034521</v>
-          </cell>
-          <cell r="F16">
-            <v>562.45612196622142</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17">
-            <v>0</v>
-          </cell>
-          <cell r="C17">
-            <v>444.24450000000007</v>
-          </cell>
-          <cell r="D17">
-            <v>557.14954360648824</v>
-          </cell>
-          <cell r="E17">
-            <v>562.16245604034521</v>
-          </cell>
-          <cell r="F17">
-            <v>562.45612196622142</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18">
-            <v>1520</v>
-          </cell>
-          <cell r="C18">
-            <v>399.82005000000009</v>
-          </cell>
-          <cell r="D18">
-            <v>557.14954360648824</v>
-          </cell>
-          <cell r="E18">
-            <v>562.16245604034521</v>
-          </cell>
-          <cell r="F18">
-            <v>562.45612196622142</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19">
-            <v>3001</v>
-          </cell>
-          <cell r="C19">
-            <v>511.83804500000008</v>
-          </cell>
-          <cell r="D19">
-            <v>538.33575499147412</v>
-          </cell>
-          <cell r="E19">
-            <v>538.97457768610138</v>
-          </cell>
-          <cell r="F19">
-            <v>539.01401076539366</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="B20">
-            <v>1001</v>
-          </cell>
-          <cell r="C20">
-            <v>760.75424050000015</v>
-          </cell>
-          <cell r="D20">
-            <v>608.90447500246023</v>
-          </cell>
-          <cell r="E20">
-            <v>610.70559409713644</v>
-          </cell>
-          <cell r="F20">
-            <v>610.8107242014878</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21">
-            <v>3000</v>
-          </cell>
-          <cell r="C21">
-            <v>784.77881645000014</v>
-          </cell>
-          <cell r="D21">
-            <v>621.00333120821699</v>
-          </cell>
-          <cell r="E21">
-            <v>622.04402670632976</v>
-          </cell>
-          <cell r="F21">
-            <v>622.10530749110842</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="B22">
-            <v>3000</v>
-          </cell>
-          <cell r="C22">
-            <v>1006.300934805</v>
-          </cell>
-          <cell r="D22">
-            <v>699.86452308823561</v>
-          </cell>
-          <cell r="E22">
-            <v>701.59326497167422</v>
-          </cell>
-          <cell r="F22">
-            <v>701.69281006389463</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23">
-            <v>2000</v>
-          </cell>
-          <cell r="C23">
-            <v>1205.6708413245001</v>
-          </cell>
-          <cell r="D23">
-            <v>781.57391099561971</v>
-          </cell>
-          <cell r="E23">
-            <v>783.57308512940529</v>
-          </cell>
-          <cell r="F23">
-            <v>783.68699065943997</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="B24">
-            <v>2000</v>
-          </cell>
-          <cell r="C24">
-            <v>1285.1037571920499</v>
-          </cell>
-          <cell r="D24">
-            <v>827.84001426797727</v>
-          </cell>
-          <cell r="E24">
-            <v>828.98236036947458</v>
-          </cell>
-          <cell r="F24">
-            <v>829.04707438582773</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="B25">
-            <v>0</v>
-          </cell>
-          <cell r="C25">
-            <v>1356.5933814728451</v>
-          </cell>
-          <cell r="D25">
-            <v>875.29269372854833</v>
-          </cell>
-          <cell r="E25">
-            <v>875.29204982069723</v>
-          </cell>
-          <cell r="F25">
-            <v>875.29173924542749</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="B26">
-            <v>0</v>
-          </cell>
-          <cell r="C26">
-            <v>1220.9340433255611</v>
-          </cell>
-          <cell r="D26">
-            <v>875.29269372854833</v>
-          </cell>
-          <cell r="E26">
-            <v>875.29204982069723</v>
-          </cell>
-          <cell r="F26">
-            <v>875.29173924542749</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="B27">
-            <v>1000</v>
-          </cell>
-          <cell r="C27">
-            <v>1098.8406389930051</v>
-          </cell>
-          <cell r="D27">
-            <v>875.29269372854833</v>
-          </cell>
-          <cell r="E27">
-            <v>875.29204982069723</v>
-          </cell>
-          <cell r="F27">
-            <v>875.29173924542749</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="B28">
-            <v>1000</v>
-          </cell>
-          <cell r="C28">
-            <v>1088.956575093704</v>
-          </cell>
-          <cell r="D28">
-            <v>810.85425648992452</v>
-          </cell>
-          <cell r="E28">
-            <v>804.92014082202627</v>
-          </cell>
-          <cell r="F28">
-            <v>804.58841372320433</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="B29">
-            <v>1000</v>
-          </cell>
-          <cell r="C29">
-            <v>1080.060917584334</v>
-          </cell>
-          <cell r="D29">
-            <v>818.83228036282014</v>
-          </cell>
-          <cell r="E29">
-            <v>811.38736224988634</v>
-          </cell>
-          <cell r="F29">
-            <v>810.97217510264068</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="B30">
-            <v>0</v>
-          </cell>
-          <cell r="C30">
-            <v>1072.0548258259009</v>
-          </cell>
-          <cell r="D30">
-            <v>826.94275080305295</v>
-          </cell>
-          <cell r="E30">
-            <v>817.9288431540798</v>
-          </cell>
-          <cell r="F30">
-            <v>817.42742312666576</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="B31">
-            <v>0</v>
-          </cell>
-          <cell r="C31">
-            <v>964.8493432433105</v>
-          </cell>
-          <cell r="D31">
-            <v>826.94275080305295</v>
-          </cell>
-          <cell r="E31">
-            <v>817.9288431540798</v>
-          </cell>
-          <cell r="F31">
-            <v>817.42742312666576</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="B32">
-            <v>0</v>
-          </cell>
-          <cell r="C32">
-            <v>868.36440891897951</v>
-          </cell>
-          <cell r="D32">
-            <v>826.94275080305295</v>
-          </cell>
-          <cell r="E32">
-            <v>817.9288431540798</v>
-          </cell>
-          <cell r="F32">
-            <v>817.42742312666576</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="B33">
-            <v>1</v>
-          </cell>
-          <cell r="C33">
-            <v>781.52796802708156</v>
-          </cell>
-          <cell r="D33">
-            <v>826.94275080305295</v>
-          </cell>
-          <cell r="E33">
-            <v>817.9288431540798</v>
-          </cell>
-          <cell r="F33">
-            <v>817.42742312666576</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="B34">
-            <v>1000</v>
-          </cell>
-          <cell r="C34">
-            <v>703.47517122437341</v>
-          </cell>
-          <cell r="D34">
-            <v>689.75373700768</v>
-          </cell>
-          <cell r="E34">
-            <v>676.15815438302445</v>
-          </cell>
-          <cell r="F34">
-            <v>675.40958448028948</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="B35">
-            <v>0</v>
-          </cell>
-          <cell r="C35">
-            <v>733.12765410193606</v>
-          </cell>
-          <cell r="D35">
-            <v>703.42495802826033</v>
-          </cell>
-          <cell r="E35">
-            <v>688.74063902231194</v>
-          </cell>
-          <cell r="F35">
-            <v>687.93364717595739</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="B36">
-            <v>3000</v>
-          </cell>
-          <cell r="C36">
-            <v>659.81488869174245</v>
-          </cell>
-          <cell r="D36">
-            <v>703.42495802826033</v>
-          </cell>
-          <cell r="E36">
-            <v>688.74063902231194</v>
-          </cell>
-          <cell r="F36">
-            <v>687.93364717595739</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="B37">
-            <v>0</v>
-          </cell>
-          <cell r="C37">
-            <v>893.83339982256825</v>
-          </cell>
-          <cell r="D37">
-            <v>774.47146486779161</v>
-          </cell>
-          <cell r="E37">
-            <v>756.95271758621516</v>
-          </cell>
-          <cell r="F37">
-            <v>755.99332939270596</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="C38">
-            <v>804.45010000000002</v>
-          </cell>
-          <cell r="D38">
-            <v>774.47149999999999</v>
-          </cell>
-          <cell r="E38">
-            <v>756.95271758621516</v>
-          </cell>
-          <cell r="F38">
-            <v>755.99332939270596</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="C39">
-            <v>804.45010000000002</v>
-          </cell>
-          <cell r="D39">
-            <v>774.47149999999999</v>
-          </cell>
-          <cell r="E39">
-            <v>756.95271758621516</v>
-          </cell>
-          <cell r="F39">
-            <v>755.99332939270596</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="C40">
-            <v>804.45010000000002</v>
-          </cell>
-          <cell r="D40">
-            <v>774.47149999999999</v>
-          </cell>
-          <cell r="E40">
-            <v>756.95271758621516</v>
-          </cell>
-          <cell r="F40">
-            <v>755.99332939270596</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="C41">
-            <v>804.45010000000002</v>
-          </cell>
-          <cell r="D41">
-            <v>774.47149999999999</v>
-          </cell>
-          <cell r="E41">
-            <v>756.95271758621516</v>
-          </cell>
-          <cell r="F41">
-            <v>755.99332939270596</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="C42">
-            <v>804.45010000000002</v>
-          </cell>
-          <cell r="D42">
-            <v>774.47149999999999</v>
-          </cell>
-          <cell r="E42">
-            <v>756.95271758621516</v>
-          </cell>
-          <cell r="F42">
-            <v>755.99332939270596</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3076,10 +2306,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="V37" sqref="V37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3497,7 +2727,7 @@
         <v>-699.24187500000005</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -3529,7 +2759,7 @@
         <v>-594.35559375000003</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -3561,7 +2791,7 @@
         <v>1014.7977453125</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -3593,7 +2823,7 @@
         <v>2343.5780835156252</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -3625,7 +2855,7 @@
         <v>-7.9586290117188128</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -3657,7 +2887,7 @@
         <v>1992.235165340039</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -3689,7 +2919,7 @@
         <v>1693.3998905390331</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -3721,7 +2951,7 @@
         <v>439.38990695817819</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -3753,7 +2983,7 @@
         <v>373.48142091445152</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -3785,7 +3015,7 @@
         <v>-1682.5407922227159</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -3817,7 +3047,7 @@
         <v>-1430.1596733893091</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -3849,7 +3079,7 @@
         <v>-215.63572238091231</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -3881,7 +3111,7 @@
         <v>-183.29036402377551</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -3913,7 +3143,7 @@
         <v>-155.7968094202092</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -3944,8 +3174,20 @@
       <c r="J30">
         <v>-1132.427288007178</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="N30" t="s">
+        <v>46</v>
+      </c>
+      <c r="O30" t="s">
+        <v>47</v>
+      </c>
+      <c r="P30" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -3976,8 +3218,23 @@
       <c r="J31">
         <v>-962.56319480610114</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M31" t="s">
+        <v>50</v>
+      </c>
+      <c r="N31" s="2">
+        <v>145.0505</v>
+      </c>
+      <c r="O31" s="2">
+        <v>313.34879999999998</v>
+      </c>
+      <c r="P31" s="2">
+        <v>317.8229</v>
+      </c>
+      <c r="Q31" s="2">
+        <v>318.20479999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -4008,8 +3265,23 @@
       <c r="J32">
         <v>-818.17871558518596</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M32" t="s">
+        <v>51</v>
+      </c>
+      <c r="N32" s="2">
+        <v>754.6798</v>
+      </c>
+      <c r="O32" s="2">
+        <v>760.08709999999996</v>
+      </c>
+      <c r="P32" s="2">
+        <v>758.64080000000001</v>
+      </c>
+      <c r="Q32" s="2">
+        <v>758.51610000000005</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -4040,8 +3312,23 @@
       <c r="J33">
         <v>-694.45190824740803</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M33" t="s">
+        <v>52</v>
+      </c>
+      <c r="N33" s="2">
+        <v>1301.6587</v>
+      </c>
+      <c r="O33" s="2">
+        <v>1278.0686000000001</v>
+      </c>
+      <c r="P33" s="2">
+        <v>1277.2547999999999</v>
+      </c>
+      <c r="Q33" s="2">
+        <v>1277.1859999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -4072,8 +3359,27 @@
       <c r="J34">
         <v>408.71587798970319</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M34" t="s">
+        <v>53</v>
+      </c>
+      <c r="N34" s="2">
+        <f>N33-N32</f>
+        <v>546.97889999999995</v>
+      </c>
+      <c r="O34" s="2">
+        <f>O33-O32</f>
+        <v>517.9815000000001</v>
+      </c>
+      <c r="P34" s="2">
+        <f>P33-P32</f>
+        <v>518.61399999999992</v>
+      </c>
+      <c r="Q34" s="2">
+        <f>Q33-Q32</f>
+        <v>518.66989999999987</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -4104,8 +3410,15 @@
       <c r="J35">
         <v>-652.59150370875227</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M35" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -4136,8 +3449,24 @@
       <c r="J36">
         <v>2445.2972218475611</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M36" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4">
+        <f>(N33-O33)/O33</f>
+        <v>1.8457616437803019E-2</v>
+      </c>
+      <c r="P36" s="4">
+        <f>(N33-P33)/P33</f>
+        <v>1.9106524399047101E-2</v>
+      </c>
+      <c r="Q36" s="4">
+        <f>(N33-Q33)/Q33</f>
+        <v>1.9161422063818451E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -4168,8 +3497,24 @@
       <c r="J37">
         <v>-921.49736142957352</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M37" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N37" s="4">
+        <f>(O33-N33)/N33</f>
+        <v>-1.8123107078683448E-2</v>
+      </c>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4">
+        <f>(O33-P33)/P33</f>
+        <v>6.3714773277824316E-4</v>
+      </c>
+      <c r="Q37" s="4">
+        <f>(O33-Q33)/Q33</f>
+        <v>6.9105048129257493E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C38">
         <v>783.27279999999996</v>
       </c>
@@ -4182,8 +3527,24 @@
       <c r="F38">
         <v>730.98243670120416</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M38" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="N38" s="4">
+        <f>(P33-N33)/N33</f>
+        <v>-1.8748309368654029E-2</v>
+      </c>
+      <c r="O38" s="4">
+        <f>(P33-O33)/O33</f>
+        <v>-6.3674203403489321E-4</v>
+      </c>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4">
+        <f>(P33-Q33)/Q33</f>
+        <v>5.3868426368602689E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C39">
         <v>783.27279999999996</v>
       </c>
@@ -4196,8 +3557,24 @@
       <c r="F39">
         <v>730.98243670120416</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M39" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="N39" s="4">
+        <f>(Q33-N33)/N33</f>
+        <v>-1.8801165005849867E-2</v>
+      </c>
+      <c r="O39" s="4">
+        <f>(Q33-O33)/O33</f>
+        <v>-6.9057326030867088E-4</v>
+      </c>
+      <c r="P39" s="4">
+        <f>(Q33-P33)/P33</f>
+        <v>-5.3865524717550633E-5</v>
+      </c>
+      <c r="Q39" s="3"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C40">
         <v>783.27279999999996</v>
       </c>
@@ -4210,8 +3587,15 @@
       <c r="F40">
         <v>730.98243670120416</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M40" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
+      <c r="P40" s="6"/>
+      <c r="Q40" s="6"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C41">
         <v>783.27279999999996</v>
       </c>
@@ -4224,8 +3608,24 @@
       <c r="F41">
         <v>730.98243670120416</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M41" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N41" s="3"/>
+      <c r="O41" s="4">
+        <f>(N32-O32)/O32</f>
+        <v>-7.1140531131234355E-3</v>
+      </c>
+      <c r="P41" s="4">
+        <f>(N32-P32)/P32</f>
+        <v>-5.2211797730889412E-3</v>
+      </c>
+      <c r="Q41" s="4">
+        <f>(N32-Q32)/Q32</f>
+        <v>-5.057638196473418E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C42">
         <v>783.27279999999996</v>
       </c>
@@ -4238,8 +3638,64 @@
       <c r="F42">
         <v>730.98243670120416</v>
       </c>
+      <c r="M42" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N42" s="4">
+        <f>(O32-N32)/N32</f>
+        <v>7.1650254849804692E-3</v>
+      </c>
+      <c r="O42" s="3"/>
+      <c r="P42" s="4">
+        <f>(O32-P32)/P32</f>
+        <v>1.9064358257556819E-3</v>
+      </c>
+      <c r="Q42" s="4">
+        <f>(O32-Q32)/Q32</f>
+        <v>2.0711491819355088E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M43" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="N43" s="4">
+        <f>(P32-N32)/N32</f>
+        <v>5.2485835714696652E-3</v>
+      </c>
+      <c r="O43" s="4">
+        <f>(P32-O32)/O32</f>
+        <v>-1.9028082439498724E-3</v>
+      </c>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="4">
+        <f>(P32-Q32)/Q32</f>
+        <v>1.6439993824779938E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M44" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="N44" s="4">
+        <f>(Q32-N32)/N32</f>
+        <v>5.0833479311358952E-3</v>
+      </c>
+      <c r="O44" s="4">
+        <f>(Q32-O32)/O32</f>
+        <v>-2.0668683891621274E-3</v>
+      </c>
+      <c r="P44" s="4">
+        <f>(Q32-P32)/P32</f>
+        <v>-1.6437291535066612E-4</v>
+      </c>
+      <c r="Q44" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="M35:Q35"/>
+    <mergeCell ref="M40:Q40"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>